<commit_message>
Fixed unesacaped chars, updated example, added requirements.txt and fixed readme
</commit_message>
<xml_diff>
--- a/example_book.xlsx
+++ b/example_book.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="446" windowWidth="24467" windowHeight="11405" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="24465" windowHeight="11400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="example_table_transactions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>name_4</t>
+  </si>
+  <si>
+    <t>BREAK ALL Ñ '\\\\ \\ // ' "'"'"</t>
   </si>
 </sst>
 </file>
@@ -131,7 +134,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -148,7 +151,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -416,9 +419,9 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.95" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -438,7 +441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.3" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -459,7 +462,7 @@
         <v>42390</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -480,7 +483,7 @@
         <v>42786</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -501,7 +504,7 @@
         <v>42237</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -522,7 +525,7 @@
         <v>42146</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -543,7 +546,7 @@
         <v>41953</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -571,15 +574,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.95" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -590,7 +593,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.3" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -601,7 +604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -612,7 +615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -623,7 +626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -631,6 +634,17 @@
         <v>11</v>
       </c>
       <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
         <v>4</v>
       </c>
     </row>

</xml_diff>